<commit_message>
commit 31-1 rate driver profile open from menu with xml File
</commit_message>
<xml_diff>
--- a/src/test/testdata/Request.xlsx
+++ b/src/test/testdata/Request.xlsx
@@ -32,10 +32,10 @@
     <t>1021132355</t>
   </si>
   <si>
-    <t>72511</t>
+    <t>72512</t>
   </si>
   <si>
-    <t>355641</t>
+    <t>355642</t>
   </si>
 </sst>
 </file>

</xml_diff>